<commit_message>
create vue demo project
</commit_message>
<xml_diff>
--- a/new install soft guide .xlsx
+++ b/new install soft guide .xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="97">
   <si>
     <t>Chrome</t>
   </si>
@@ -255,12 +255,6 @@
   </si>
   <si>
     <t>test connect,open git bash</t>
-  </si>
-  <si>
-    <t>ssh-add -l</t>
-  </si>
-  <si>
-    <t>ssh-add -l -E md5</t>
   </si>
   <si>
     <t>clip &lt; C:/Users/dqi/.ssh/id_rsa.pub</t>
@@ -324,7 +318,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,16 +346,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,12 +357,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -430,7 +410,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1014,10 +993,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D61"/>
+  <dimension ref="A2:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1032,12 +1011,12 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1058,7 +1037,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1066,92 +1045,88 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="12" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="12" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>3</v>
-      </c>
-      <c r="B39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>4</v>
-      </c>
-      <c r="B43" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="11" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>5</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="10" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
-        <v>83</v>
-      </c>
-      <c r="C50" s="10" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="B53" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1169,37 +1144,27 @@
       <c r="B56" t="s">
         <v>90</v>
       </c>
+      <c r="C56" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B58" t="s">
         <v>92</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C57" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B59" t="s">
+      <c r="A59" t="s">
         <v>94</v>
-      </c>
-      <c r="C59" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C47" r:id="rId1"/>
-    <hyperlink ref="C50" r:id="rId2"/>
+    <hyperlink ref="C45" r:id="rId1"/>
+    <hyperlink ref="C48" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
add multiuser git config
</commit_message>
<xml_diff>
--- a/new install soft guide .xlsx
+++ b/new install soft guide .xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
   <si>
     <t>Chrome</t>
   </si>
@@ -257,6 +257,12 @@
     <t>test connect,open git bash</t>
   </si>
   <si>
+    <t>ssh-add -l</t>
+  </si>
+  <si>
+    <t>ssh-add -l -E md5</t>
+  </si>
+  <si>
     <t>clip &lt; C:/Users/dqi/.ssh/id_rsa.pub</t>
   </si>
   <si>
@@ -312,13 +318,19 @@
   </si>
   <si>
     <t>git config --global user.email "qidawei01@qq.com"</t>
+  </si>
+  <si>
+    <t>https://www.cnblogs.com/xjnotxj/p/5845574.html</t>
+  </si>
+  <si>
+    <t>Multiuser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,8 +358,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +377,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,7 +415,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -410,6 +436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -438,8 +465,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>38134</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>563914</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>53760</xdr:rowOff>
     </xdr:to>
@@ -993,13 +1020,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C59"/>
+  <dimension ref="A2:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1011,12 +1041,12 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1037,7 +1067,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1045,88 +1075,100 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>3</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
         <v>4</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
         <v>5</v>
       </c>
-      <c r="B45" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="10" t="s">
+      <c r="C47" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>86</v>
+        <v>100</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
+      <c r="A53" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1144,31 +1186,42 @@
       <c r="B56" t="s">
         <v>90</v>
       </c>
-      <c r="C56" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
         <v>92</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="B59" t="s">
         <v>94</v>
+      </c>
+      <c r="C59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C45" r:id="rId1"/>
-    <hyperlink ref="C48" r:id="rId2"/>
+    <hyperlink ref="C47" r:id="rId1"/>
+    <hyperlink ref="C50" r:id="rId2"/>
+    <hyperlink ref="C52" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>